<commit_message>
Lightweighting of components was not properly applied
The lightweighting was only applied to the glider, not the other components when building the inventories.
</commit_message>
<xml_diff>
--- a/dev/Input data_truck.xlsx
+++ b/dev/Input data_truck.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="23040" windowHeight="9024" tabRatio="518"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="23040" windowHeight="9030" tabRatio="518"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle parameters" sheetId="22" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="248">
   <si>
     <t>power to mass ratio</t>
   </si>
@@ -782,6 +782,9 @@
   <si>
     <t>32t, 40t, 60t</t>
   </si>
+  <si>
+    <t>own assumption for 2000, 2010, 2050. Cox et al. 2020 for 2020, 2040. Assumed to be half that of passenger cars.</t>
+  </si>
 </sst>
 </file>
 
@@ -1310,30 +1313,30 @@
       <pane xSplit="11" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E264" sqref="E264"/>
+      <selection pane="bottomRight" activeCell="N304" sqref="N304"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.21875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="37.77734375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="38.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" style="20" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="20" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="2" customWidth="1"/>
-    <col min="10" max="10" width="33.5546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="18" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.21875" style="1"/>
+    <col min="22" max="23" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>134</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L2" s="19" t="s">
         <v>12</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -2100,7 +2103,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -2201,7 +2204,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -2266,7 +2269,7 @@
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
     </row>
-    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -2339,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -2549,7 +2552,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="14.7" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="14.65" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -2759,7 +2762,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="14.7" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="14.65" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -2860,7 +2863,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -2961,7 +2964,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="18" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
@@ -3151,7 +3154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
@@ -3253,7 +3256,7 @@
         <v>943.11249999999995</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
@@ -3355,7 +3358,7 @@
         <v>1886.2249999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -3457,7 +3460,7 @@
         <v>3600.9749999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -3559,7 +3562,7 @@
         <v>3772.45</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -3661,7 +3664,7 @@
         <v>4115.3999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:30" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
@@ -3763,7 +3766,7 @@
         <v>4115.3999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -3865,7 +3868,7 @@
         <v>5658.6750000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>57</v>
       </c>
@@ -3966,7 +3969,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>57</v>
       </c>
@@ -4067,7 +4070,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
@@ -4168,7 +4171,7 @@
         <v>2.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>57</v>
       </c>
@@ -4269,7 +4272,7 @@
         <v>6.1199999999999991E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>57</v>
       </c>
@@ -4371,7 +4374,7 @@
       </c>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>57</v>
       </c>
@@ -4473,7 +4476,7 @@
       </c>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
@@ -4575,7 +4578,7 @@
       </c>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>57</v>
       </c>
@@ -4657,7 +4660,7 @@
       </c>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -4739,7 +4742,7 @@
       </c>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
@@ -4821,7 +4824,7 @@
       </c>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
@@ -4903,7 +4906,7 @@
       </c>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -4985,7 +4988,7 @@
       </c>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>57</v>
       </c>
@@ -5067,7 +5070,7 @@
       </c>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
@@ -5149,7 +5152,7 @@
       </c>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -5257,7 +5260,7 @@
       </c>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
@@ -5365,7 +5368,7 @@
       </c>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -5473,7 +5476,7 @@
       </c>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -5581,7 +5584,7 @@
       </c>
       <c r="AD44" s="1"/>
     </row>
-    <row r="45" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>57</v>
       </c>
@@ -5689,7 +5692,7 @@
       </c>
       <c r="AD45" s="1"/>
     </row>
-    <row r="46" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
@@ -5797,7 +5800,7 @@
       </c>
       <c r="AD46" s="1"/>
     </row>
-    <row r="47" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>57</v>
       </c>
@@ -5905,7 +5908,7 @@
       </c>
       <c r="AD47" s="1"/>
     </row>
-    <row r="48" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
@@ -6013,7 +6016,7 @@
       </c>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
@@ -6121,7 +6124,7 @@
       </c>
       <c r="AD49" s="1"/>
     </row>
-    <row r="50" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -6229,7 +6232,7 @@
       </c>
       <c r="AD50" s="1"/>
     </row>
-    <row r="51" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -6337,7 +6340,7 @@
       </c>
       <c r="AD51" s="1"/>
     </row>
-    <row r="52" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
@@ -6445,7 +6448,7 @@
       </c>
       <c r="AD52" s="1"/>
     </row>
-    <row r="53" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>57</v>
       </c>
@@ -6553,7 +6556,7 @@
       </c>
       <c r="AD53" s="1"/>
     </row>
-    <row r="54" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -6661,7 +6664,7 @@
       </c>
       <c r="AD54" s="1"/>
     </row>
-    <row r="55" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>57</v>
       </c>
@@ -6751,7 +6754,7 @@
       </c>
       <c r="AD55" s="1"/>
     </row>
-    <row r="56" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -6841,7 +6844,7 @@
       </c>
       <c r="AD56" s="1"/>
     </row>
-    <row r="57" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>57</v>
       </c>
@@ -6931,7 +6934,7 @@
       </c>
       <c r="AD57" s="1"/>
     </row>
-    <row r="58" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -7021,7 +7024,7 @@
       </c>
       <c r="AD58" s="1"/>
     </row>
-    <row r="59" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -7111,7 +7114,7 @@
       </c>
       <c r="AD59" s="1"/>
     </row>
-    <row r="60" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -7201,7 +7204,7 @@
       </c>
       <c r="AD60" s="1"/>
     </row>
-    <row r="61" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
@@ -7291,7 +7294,7 @@
       </c>
       <c r="AD61" s="1"/>
     </row>
-    <row r="62" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>57</v>
       </c>
@@ -7373,7 +7376,7 @@
       </c>
       <c r="AD62" s="1"/>
     </row>
-    <row r="63" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>57</v>
       </c>
@@ -7463,7 +7466,7 @@
       </c>
       <c r="AD63" s="1"/>
     </row>
-    <row r="64" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>57</v>
       </c>
@@ -7553,7 +7556,7 @@
       </c>
       <c r="AD64" s="1"/>
     </row>
-    <row r="65" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>57</v>
       </c>
@@ -7643,7 +7646,7 @@
       </c>
       <c r="AD65" s="1"/>
     </row>
-    <row r="66" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>57</v>
       </c>
@@ -7733,7 +7736,7 @@
       </c>
       <c r="AD66" s="1"/>
     </row>
-    <row r="67" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>57</v>
       </c>
@@ -7823,7 +7826,7 @@
       </c>
       <c r="AD67" s="1"/>
     </row>
-    <row r="68" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>57</v>
       </c>
@@ -7913,7 +7916,7 @@
       </c>
       <c r="AD68" s="1"/>
     </row>
-    <row r="69" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>57</v>
       </c>
@@ -8003,7 +8006,7 @@
       </c>
       <c r="AD69" s="1"/>
     </row>
-    <row r="70" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>57</v>
       </c>
@@ -8085,7 +8088,7 @@
       </c>
       <c r="AD70" s="1"/>
     </row>
-    <row r="71" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>57</v>
       </c>
@@ -8167,7 +8170,7 @@
       </c>
       <c r="AD71" s="1"/>
     </row>
-    <row r="72" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>57</v>
       </c>
@@ -8255,7 +8258,7 @@
       </c>
       <c r="AD72" s="1"/>
     </row>
-    <row r="73" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>57</v>
       </c>
@@ -8337,7 +8340,7 @@
       </c>
       <c r="AD73" s="1"/>
     </row>
-    <row r="74" spans="1:30" s="24" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
@@ -8445,7 +8448,7 @@
       </c>
       <c r="AD74" s="1"/>
     </row>
-    <row r="75" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
@@ -8527,7 +8530,7 @@
       </c>
       <c r="AD75" s="1"/>
     </row>
-    <row r="76" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>57</v>
       </c>
@@ -8609,7 +8612,7 @@
       </c>
       <c r="AD76" s="1"/>
     </row>
-    <row r="77" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>57</v>
       </c>
@@ -8691,7 +8694,7 @@
       </c>
       <c r="AD77" s="1"/>
     </row>
-    <row r="78" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>57</v>
       </c>
@@ -8773,7 +8776,7 @@
       </c>
       <c r="AD78" s="1"/>
     </row>
-    <row r="79" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>57</v>
       </c>
@@ -8855,7 +8858,7 @@
       </c>
       <c r="AD79" s="1"/>
     </row>
-    <row r="80" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>57</v>
       </c>
@@ -8937,7 +8940,7 @@
       </c>
       <c r="AD80" s="1"/>
     </row>
-    <row r="81" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>57</v>
       </c>
@@ -9019,7 +9022,7 @@
       </c>
       <c r="AD81" s="1"/>
     </row>
-    <row r="82" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>57</v>
       </c>
@@ -9077,7 +9080,7 @@
       </c>
       <c r="AD82" s="1"/>
     </row>
-    <row r="83" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>57</v>
       </c>
@@ -9159,7 +9162,7 @@
       </c>
       <c r="AD83" s="1"/>
     </row>
-    <row r="84" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>57</v>
       </c>
@@ -9241,7 +9244,7 @@
       </c>
       <c r="AD84" s="1"/>
     </row>
-    <row r="85" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>57</v>
       </c>
@@ -9323,7 +9326,7 @@
       </c>
       <c r="AD85" s="1"/>
     </row>
-    <row r="86" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>57</v>
       </c>
@@ -9405,7 +9408,7 @@
       </c>
       <c r="AD86" s="1"/>
     </row>
-    <row r="87" spans="1:30" s="24" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>57</v>
       </c>
@@ -9495,7 +9498,7 @@
       </c>
       <c r="AD87" s="1"/>
     </row>
-    <row r="88" spans="1:30" s="24" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>57</v>
       </c>
@@ -9585,7 +9588,7 @@
       </c>
       <c r="AD88" s="1"/>
     </row>
-    <row r="89" spans="1:30" s="24" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>57</v>
       </c>
@@ -9675,7 +9678,7 @@
       </c>
       <c r="AD89" s="1"/>
     </row>
-    <row r="90" spans="1:30" s="24" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>57</v>
       </c>
@@ -9765,7 +9768,7 @@
       </c>
       <c r="AD90" s="1"/>
     </row>
-    <row r="91" spans="1:30" s="24" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>57</v>
       </c>
@@ -9855,7 +9858,7 @@
       </c>
       <c r="AD91" s="1"/>
     </row>
-    <row r="92" spans="1:30" s="24" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>57</v>
       </c>
@@ -9945,7 +9948,7 @@
       </c>
       <c r="AD92" s="1"/>
     </row>
-    <row r="93" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>57</v>
       </c>
@@ -10027,7 +10030,7 @@
       </c>
       <c r="AD93" s="1"/>
     </row>
-    <row r="94" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>57</v>
       </c>
@@ -10114,7 +10117,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="95" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>35</v>
       </c>
@@ -10215,7 +10218,7 @@
         <v>180000</v>
       </c>
     </row>
-    <row r="96" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>35</v>
       </c>
@@ -10316,7 +10319,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="97" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>35</v>
       </c>
@@ -10417,7 +10420,7 @@
         <v>1050000</v>
       </c>
     </row>
-    <row r="98" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>35</v>
       </c>
@@ -10518,7 +10521,7 @@
         <v>875000</v>
       </c>
     </row>
-    <row r="99" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>35</v>
       </c>
@@ -10619,7 +10622,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="100" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>35</v>
       </c>
@@ -10720,7 +10723,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="101" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>35</v>
       </c>
@@ -10821,7 +10824,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="102" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>35</v>
       </c>
@@ -10922,7 +10925,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="103" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>35</v>
       </c>
@@ -11023,7 +11026,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="104" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>35</v>
       </c>
@@ -11124,7 +11127,7 @@
         <v>52500</v>
       </c>
     </row>
-    <row r="105" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>35</v>
       </c>
@@ -11225,7 +11228,7 @@
         <v>43750</v>
       </c>
     </row>
-    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>35</v>
       </c>
@@ -11326,7 +11329,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="107" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>35</v>
       </c>
@@ -11427,7 +11430,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="108" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>35</v>
       </c>
@@ -11528,7 +11531,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="109" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>37</v>
       </c>
@@ -11615,7 +11618,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="110" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>37</v>
       </c>
@@ -11706,7 +11709,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="111" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>37</v>
       </c>
@@ -11791,7 +11794,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="112" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>37</v>
       </c>
@@ -11876,7 +11879,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>30</v>
       </c>
@@ -11937,7 +11940,7 @@
       <c r="AB113" s="5"/>
       <c r="AC113" s="5"/>
     </row>
-    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>30</v>
       </c>
@@ -11998,7 +12001,7 @@
       <c r="AB114" s="5"/>
       <c r="AC114" s="5"/>
     </row>
-    <row r="115" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>30</v>
       </c>
@@ -12059,7 +12062,7 @@
       <c r="AB115" s="5"/>
       <c r="AC115" s="5"/>
     </row>
-    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>30</v>
       </c>
@@ -12148,7 +12151,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>30</v>
       </c>
@@ -12233,7 +12236,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="118" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>30</v>
       </c>
@@ -12322,7 +12325,7 @@
         <v>27500</v>
       </c>
     </row>
-    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>30</v>
       </c>
@@ -12407,7 +12410,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>30</v>
       </c>
@@ -12496,7 +12499,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>30</v>
       </c>
@@ -12585,7 +12588,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>30</v>
       </c>
@@ -12684,7 +12687,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>30</v>
       </c>
@@ -12783,7 +12786,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>30</v>
       </c>
@@ -12885,7 +12888,7 @@
         <v>11646.250000000004</v>
       </c>
     </row>
-    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>30</v>
       </c>
@@ -12987,7 +12990,7 @@
         <v>11646.250000000004</v>
       </c>
     </row>
-    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>30</v>
       </c>
@@ -13076,7 +13079,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>30</v>
       </c>
@@ -13171,7 +13174,7 @@
         <v>0.94760000000000011</v>
       </c>
     </row>
-    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>30</v>
       </c>
@@ -13266,7 +13269,7 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>30</v>
       </c>
@@ -13355,7 +13358,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>30</v>
       </c>
@@ -13444,7 +13447,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>30</v>
       </c>
@@ -13533,7 +13536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>30</v>
       </c>
@@ -13622,7 +13625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>30</v>
       </c>
@@ -13717,7 +13720,7 @@
         <v>3.4499999999999997</v>
       </c>
     </row>
-    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>30</v>
       </c>
@@ -13806,7 +13809,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>30</v>
       </c>
@@ -13895,7 +13898,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>30</v>
       </c>
@@ -13984,7 +13987,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>30</v>
       </c>
@@ -14071,7 +14074,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>30</v>
       </c>
@@ -14158,7 +14161,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>30</v>
       </c>
@@ -14257,7 +14260,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>30</v>
       </c>
@@ -14356,7 +14359,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="23" t="s">
         <v>27</v>
       </c>
@@ -14418,7 +14421,7 @@
       <c r="AB141" s="19"/>
       <c r="AC141" s="19"/>
     </row>
-    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="23" t="s">
         <v>27</v>
       </c>
@@ -14480,7 +14483,7 @@
       <c r="AB142" s="19"/>
       <c r="AC142" s="19"/>
     </row>
-    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="23" t="s">
         <v>27</v>
       </c>
@@ -14542,7 +14545,7 @@
       <c r="AB143" s="19"/>
       <c r="AC143" s="19"/>
     </row>
-    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23" t="s">
         <v>27</v>
       </c>
@@ -14604,7 +14607,7 @@
       <c r="AB144" s="19"/>
       <c r="AC144" s="19"/>
     </row>
-    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="23" t="s">
         <v>27</v>
       </c>
@@ -14666,7 +14669,7 @@
       <c r="AB145" s="19"/>
       <c r="AC145" s="19"/>
     </row>
-    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="23" t="s">
         <v>27</v>
       </c>
@@ -14728,7 +14731,7 @@
       <c r="AB146" s="19"/>
       <c r="AC146" s="19"/>
     </row>
-    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="23" t="s">
         <v>27</v>
       </c>
@@ -14790,7 +14793,7 @@
       <c r="AB147" s="19"/>
       <c r="AC147" s="19"/>
     </row>
-    <row r="148" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="23" t="s">
         <v>27</v>
       </c>
@@ -14891,7 +14894,7 @@
         <v>242.5</v>
       </c>
     </row>
-    <row r="149" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="23" t="s">
         <v>27</v>
       </c>
@@ -14992,7 +14995,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="23" t="s">
         <v>27</v>
       </c>
@@ -15093,7 +15096,7 @@
         <v>1247.5</v>
       </c>
     </row>
-    <row r="151" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="23" t="s">
         <v>27</v>
       </c>
@@ -15194,7 +15197,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="152" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="23" t="s">
         <v>27</v>
       </c>
@@ -15295,7 +15298,7 @@
         <v>1422.5</v>
       </c>
     </row>
-    <row r="153" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="23" t="s">
         <v>27</v>
       </c>
@@ -15396,7 +15399,7 @@
         <v>1777.5</v>
       </c>
     </row>
-    <row r="154" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="23" t="s">
         <v>27</v>
       </c>
@@ -15497,7 +15500,7 @@
         <v>2666.25</v>
       </c>
     </row>
-    <row r="155" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="23" t="s">
         <v>27</v>
       </c>
@@ -15598,7 +15601,7 @@
         <v>387.5</v>
       </c>
     </row>
-    <row r="156" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="23" t="s">
         <v>27</v>
       </c>
@@ -15699,7 +15702,7 @@
         <v>831.25</v>
       </c>
     </row>
-    <row r="157" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="23" t="s">
         <v>27</v>
       </c>
@@ -15800,7 +15803,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="158" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="23" t="s">
         <v>27</v>
       </c>
@@ -15901,7 +15904,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="159" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="23" t="s">
         <v>27</v>
       </c>
@@ -16002,7 +16005,7 @@
         <v>2656.25</v>
       </c>
     </row>
-    <row r="160" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="23" t="s">
         <v>27</v>
       </c>
@@ -16103,7 +16106,7 @@
         <v>3320</v>
       </c>
     </row>
-    <row r="161" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="23" t="s">
         <v>27</v>
       </c>
@@ -16204,7 +16207,7 @@
         <v>4980</v>
       </c>
     </row>
-    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="23" t="s">
         <v>27</v>
       </c>
@@ -16291,7 +16294,7 @@
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="23" t="s">
         <v>27</v>
       </c>
@@ -16380,7 +16383,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="23" t="s">
         <v>27</v>
       </c>
@@ -16469,7 +16472,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="23" t="s">
         <v>27</v>
       </c>
@@ -16558,7 +16561,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="23" t="s">
         <v>27</v>
       </c>
@@ -16647,7 +16650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="23" t="s">
         <v>27</v>
       </c>
@@ -16736,7 +16739,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="23" t="s">
         <v>27</v>
       </c>
@@ -16825,7 +16828,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="23" t="s">
         <v>27</v>
       </c>
@@ -16914,7 +16917,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="23" t="s">
         <v>27</v>
       </c>
@@ -17021,7 +17024,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="23" t="s">
         <v>27</v>
       </c>
@@ -17128,7 +17131,7 @@
         <v>34.4</v>
       </c>
     </row>
-    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="23" t="s">
         <v>27</v>
       </c>
@@ -17229,7 +17232,7 @@
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="23" t="s">
         <v>27</v>
       </c>
@@ -17330,7 +17333,7 @@
         <v>31.200000000000003</v>
       </c>
     </row>
-    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="23" t="s">
         <v>27</v>
       </c>
@@ -17431,7 +17434,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="175" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="23" t="s">
         <v>27</v>
       </c>
@@ -17532,7 +17535,7 @@
         <v>26.400000000000002</v>
       </c>
     </row>
-    <row r="176" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="23" t="s">
         <v>27</v>
       </c>
@@ -17633,7 +17636,7 @@
         <v>19.200000000000003</v>
       </c>
     </row>
-    <row r="177" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="23" t="s">
         <v>27</v>
       </c>
@@ -17734,7 +17737,7 @@
         <v>823.75</v>
       </c>
     </row>
-    <row r="178" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="23" t="s">
         <v>27</v>
       </c>
@@ -17835,7 +17838,7 @@
         <v>1766.25</v>
       </c>
     </row>
-    <row r="179" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="23" t="s">
         <v>27</v>
       </c>
@@ -17936,7 +17939,7 @@
         <v>2875</v>
       </c>
     </row>
-    <row r="180" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="23" t="s">
         <v>27</v>
       </c>
@@ -18037,7 +18040,7 @@
         <v>3125</v>
       </c>
     </row>
-    <row r="181" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="23" t="s">
         <v>27</v>
       </c>
@@ -18138,7 +18141,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="182" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="23" t="s">
         <v>27</v>
       </c>
@@ -18239,7 +18242,7 @@
         <v>3375</v>
       </c>
     </row>
-    <row r="183" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="23" t="s">
         <v>27</v>
       </c>
@@ -18340,7 +18343,7 @@
         <v>5062.5</v>
       </c>
     </row>
-    <row r="184" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="23" t="s">
         <v>27</v>
       </c>
@@ -18429,7 +18432,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="23" t="s">
         <v>27</v>
       </c>
@@ -18518,7 +18521,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="186" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="23" t="s">
         <v>27</v>
       </c>
@@ -18607,7 +18610,7 @@
         <v>10900</v>
       </c>
     </row>
-    <row r="187" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="23" t="s">
         <v>27</v>
       </c>
@@ -18696,7 +18699,7 @@
         <v>16400</v>
       </c>
     </row>
-    <row r="188" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="23" t="s">
         <v>27</v>
       </c>
@@ -18785,7 +18788,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="23" t="s">
         <v>27</v>
       </c>
@@ -18874,7 +18877,7 @@
         <v>28100</v>
       </c>
     </row>
-    <row r="190" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="23" t="s">
         <v>27</v>
       </c>
@@ -18963,7 +18966,7 @@
         <v>39000</v>
       </c>
     </row>
-    <row r="191" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="23" t="s">
         <v>27</v>
       </c>
@@ -19060,7 +19063,7 @@
         <v>0.35000000000000003</v>
       </c>
     </row>
-    <row r="192" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="23" t="s">
         <v>27</v>
       </c>
@@ -19157,7 +19160,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="193" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>27</v>
       </c>
@@ -19218,7 +19221,7 @@
       <c r="AB193" s="4"/>
       <c r="AC193" s="4"/>
     </row>
-    <row r="194" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>27</v>
       </c>
@@ -19279,7 +19282,7 @@
       <c r="AB194" s="4"/>
       <c r="AC194" s="4"/>
     </row>
-    <row r="195" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>27</v>
       </c>
@@ -19340,7 +19343,7 @@
       <c r="AB195" s="4"/>
       <c r="AC195" s="4"/>
     </row>
-    <row r="196" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>27</v>
       </c>
@@ -19401,7 +19404,7 @@
       <c r="AB196" s="4"/>
       <c r="AC196" s="4"/>
     </row>
-    <row r="197" spans="1:29" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:29" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>27</v>
       </c>
@@ -19462,7 +19465,7 @@
       <c r="AB197" s="4"/>
       <c r="AC197" s="4"/>
     </row>
-    <row r="198" spans="1:29" ht="29.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:29" ht="29.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>27</v>
       </c>
@@ -19523,7 +19526,7 @@
       <c r="AB198" s="4"/>
       <c r="AC198" s="4"/>
     </row>
-    <row r="199" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>27</v>
       </c>
@@ -19584,7 +19587,7 @@
       <c r="AB199" s="4"/>
       <c r="AC199" s="4"/>
     </row>
-    <row r="200" spans="1:29" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:29" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="23" t="s">
         <v>27</v>
       </c>
@@ -19685,7 +19688,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="201" spans="1:29" ht="26.7" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:29" ht="26.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="23" t="s">
         <v>27</v>
       </c>
@@ -19786,7 +19789,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="202" spans="1:29" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:29" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="23" t="s">
         <v>27</v>
       </c>
@@ -19887,7 +19890,7 @@
         <v>768.75</v>
       </c>
     </row>
-    <row r="203" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="23" t="s">
         <v>27</v>
       </c>
@@ -19988,7 +19991,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="204" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="23" t="s">
         <v>27</v>
       </c>
@@ -20053,7 +20056,7 @@
       <c r="AB204" s="13"/>
       <c r="AC204" s="13"/>
     </row>
-    <row r="205" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="23" t="s">
         <v>27</v>
       </c>
@@ -20154,7 +20157,7 @@
         <v>4298.75</v>
       </c>
     </row>
-    <row r="206" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="23" t="s">
         <v>27</v>
       </c>
@@ -20255,7 +20258,7 @@
         <v>6448.75</v>
       </c>
     </row>
-    <row r="207" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="23" t="s">
         <v>27</v>
       </c>
@@ -20353,7 +20356,7 @@
         <v>3.8581874999999992</v>
       </c>
     </row>
-    <row r="208" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="23" t="s">
         <v>27</v>
       </c>
@@ -20451,7 +20454,7 @@
         <v>5.4871999999999996</v>
       </c>
     </row>
-    <row r="209" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="23" t="s">
         <v>27</v>
       </c>
@@ -20549,7 +20552,7 @@
         <v>6.6875249999999982</v>
       </c>
     </row>
-    <row r="210" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="23" t="s">
         <v>27</v>
       </c>
@@ -20647,7 +20650,7 @@
         <v>6.6875249999999982</v>
       </c>
     </row>
-    <row r="211" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="23" t="s">
         <v>27</v>
       </c>
@@ -20736,7 +20739,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="212" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="23" t="s">
         <v>27</v>
       </c>
@@ -20834,7 +20837,7 @@
         <v>7.2019499999999992</v>
       </c>
     </row>
-    <row r="213" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="23" t="s">
         <v>27</v>
       </c>
@@ -20932,7 +20935,7 @@
         <v>7.2019499999999992</v>
       </c>
     </row>
-    <row r="214" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="23" t="s">
         <v>27</v>
       </c>
@@ -21033,7 +21036,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="215" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="23" t="s">
         <v>27</v>
       </c>
@@ -21134,7 +21137,7 @@
         <v>117.5</v>
       </c>
     </row>
-    <row r="216" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="23" t="s">
         <v>27</v>
       </c>
@@ -21235,7 +21238,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="217" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="23" t="s">
         <v>27</v>
       </c>
@@ -21336,7 +21339,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="218" spans="1:29" ht="15.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:29" ht="15.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="23" t="s">
         <v>27</v>
       </c>
@@ -21437,7 +21440,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="219" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="23" t="s">
         <v>27</v>
       </c>
@@ -21538,7 +21541,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="220" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="23" t="s">
         <v>27</v>
       </c>
@@ -21639,7 +21642,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="221" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="23" t="s">
         <v>27</v>
       </c>
@@ -21740,7 +21743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="222" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="23" t="s">
         <v>27</v>
       </c>
@@ -21841,7 +21844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="223" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="23" t="s">
         <v>27</v>
       </c>
@@ -21942,7 +21945,7 @@
         <v>156.25</v>
       </c>
     </row>
-    <row r="224" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="23" t="s">
         <v>27</v>
       </c>
@@ -22043,7 +22046,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="225" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="23" t="s">
         <v>27</v>
       </c>
@@ -22144,7 +22147,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="226" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="23" t="s">
         <v>27</v>
       </c>
@@ -22245,7 +22248,7 @@
         <v>331.25</v>
       </c>
     </row>
-    <row r="227" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="23" t="s">
         <v>27</v>
       </c>
@@ -22346,7 +22349,7 @@
         <v>497.5</v>
       </c>
     </row>
-    <row r="228" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="23" t="s">
         <v>27</v>
       </c>
@@ -22447,7 +22450,7 @@
         <v>0.37400000000000005</v>
       </c>
     </row>
-    <row r="229" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="23" t="s">
         <v>27</v>
       </c>
@@ -22548,7 +22551,7 @@
         <v>0.22000000000000003</v>
       </c>
     </row>
-    <row r="230" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>27</v>
       </c>
@@ -22649,7 +22652,7 @@
         <v>0.35200000000000004</v>
       </c>
     </row>
-    <row r="231" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>27</v>
       </c>
@@ -22750,7 +22753,7 @@
         <v>0.50600000000000012</v>
       </c>
     </row>
-    <row r="232" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>27</v>
       </c>
@@ -22851,7 +22854,7 @@
         <v>0.49500000000000005</v>
       </c>
     </row>
-    <row r="233" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>27</v>
       </c>
@@ -22952,7 +22955,7 @@
         <v>0.38500000000000001</v>
       </c>
     </row>
-    <row r="234" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>27</v>
       </c>
@@ -23053,7 +23056,7 @@
         <v>0.38500000000000001</v>
       </c>
     </row>
-    <row r="235" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="23" t="s">
         <v>27</v>
       </c>
@@ -23154,7 +23157,7 @@
         <v>218.75</v>
       </c>
     </row>
-    <row r="236" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="23" t="s">
         <v>27</v>
       </c>
@@ -23255,7 +23258,7 @@
         <v>468.75</v>
       </c>
     </row>
-    <row r="237" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="23" t="s">
         <v>27</v>
       </c>
@@ -23356,7 +23359,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="238" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="23" t="s">
         <v>27</v>
       </c>
@@ -23457,7 +23460,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="239" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="23" t="s">
         <v>27</v>
       </c>
@@ -23558,7 +23561,7 @@
         <v>1152.5</v>
       </c>
     </row>
-    <row r="240" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="23" t="s">
         <v>27</v>
       </c>
@@ -23659,7 +23662,7 @@
         <v>1441.25</v>
       </c>
     </row>
-    <row r="241" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="23" t="s">
         <v>27</v>
       </c>
@@ -23760,7 +23763,7 @@
         <v>2162.5</v>
       </c>
     </row>
-    <row r="242" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="23" t="s">
         <v>27</v>
       </c>
@@ -23861,7 +23864,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="243" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="23" t="s">
         <v>27</v>
       </c>
@@ -23962,7 +23965,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="244" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="23" t="s">
         <v>27</v>
       </c>
@@ -24063,7 +24066,7 @@
         <v>156.25</v>
       </c>
     </row>
-    <row r="245" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="23" t="s">
         <v>27</v>
       </c>
@@ -24164,7 +24167,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="246" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="23" t="s">
         <v>27</v>
       </c>
@@ -24265,7 +24268,7 @@
         <v>783.75</v>
       </c>
     </row>
-    <row r="247" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="23" t="s">
         <v>27</v>
       </c>
@@ -24366,7 +24369,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="248" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="23" t="s">
         <v>27</v>
       </c>
@@ -24467,7 +24470,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="249" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="23" t="s">
         <v>27</v>
       </c>
@@ -24530,7 +24533,7 @@
       <c r="AB249" s="5"/>
       <c r="AC249" s="5"/>
     </row>
-    <row r="250" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="23" t="s">
         <v>27</v>
       </c>
@@ -24617,7 +24620,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="251" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="23" t="s">
         <v>27</v>
       </c>
@@ -24704,7 +24707,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="252" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
         <v>28</v>
       </c>
@@ -24793,7 +24796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="253" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
         <v>28</v>
       </c>
@@ -24894,7 +24897,7 @@
         <v>161.25</v>
       </c>
     </row>
-    <row r="254" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>28</v>
       </c>
@@ -24991,7 +24994,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="255" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>28</v>
       </c>
@@ -25086,7 +25089,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="256" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>28</v>
       </c>
@@ -25179,7 +25182,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="257" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>28</v>
       </c>
@@ -25276,7 +25279,7 @@
         <v>5.5000000000000007E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
         <v>28</v>
       </c>
@@ -25379,7 +25382,7 @@
         <v>5.5000000000000007E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:29" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:29" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>28</v>
       </c>
@@ -25468,7 +25471,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="260" spans="1:29" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:29" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
         <v>28</v>
       </c>
@@ -25575,7 +25578,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="261" spans="1:29" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:29" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>28</v>
       </c>
@@ -25604,67 +25607,67 @@
         <v>82</v>
       </c>
       <c r="J261" s="3" t="s">
-        <v>147</v>
+        <v>247</v>
       </c>
       <c r="K261" s="3" t="s">
         <v>69</v>
       </c>
       <c r="L261" s="5">
+        <v>350</v>
+      </c>
+      <c r="M261" s="5">
+        <v>250</v>
+      </c>
+      <c r="N261" s="5">
+        <v>450</v>
+      </c>
+      <c r="O261" s="5">
+        <v>400</v>
+      </c>
+      <c r="P261" s="5">
+        <v>300</v>
+      </c>
+      <c r="Q261" s="5">
+        <v>500</v>
+      </c>
+      <c r="R261" s="5">
+        <v>450</v>
+      </c>
+      <c r="S261" s="5">
+        <v>350</v>
+      </c>
+      <c r="T261" s="5">
+        <v>550</v>
+      </c>
+      <c r="U261" s="5">
+        <v>450</v>
+      </c>
+      <c r="V261" s="5">
+        <v>350</v>
+      </c>
+      <c r="W261" s="5">
+        <v>550</v>
+      </c>
+      <c r="X261" s="5">
+        <v>500</v>
+      </c>
+      <c r="Y261" s="5">
+        <v>400</v>
+      </c>
+      <c r="Z261" s="5">
+        <v>600</v>
+      </c>
+      <c r="AA261" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB261" s="3">
+        <v>550</v>
+      </c>
+      <c r="AC261" s="3">
         <v>700</v>
       </c>
-      <c r="M261" s="5">
-        <v>500</v>
-      </c>
-      <c r="N261" s="5">
-        <v>900</v>
-      </c>
-      <c r="O261" s="5">
-        <v>800</v>
-      </c>
-      <c r="P261" s="5">
-        <v>600</v>
-      </c>
-      <c r="Q261" s="5">
-        <v>1000</v>
-      </c>
-      <c r="R261" s="5">
-        <v>900</v>
-      </c>
-      <c r="S261" s="5">
-        <v>700</v>
-      </c>
-      <c r="T261" s="5">
-        <v>1100</v>
-      </c>
-      <c r="U261" s="5">
-        <v>900</v>
-      </c>
-      <c r="V261" s="5">
-        <v>700</v>
-      </c>
-      <c r="W261" s="5">
-        <v>1100</v>
-      </c>
-      <c r="X261" s="5">
-        <v>1000</v>
-      </c>
-      <c r="Y261" s="5">
-        <v>800</v>
-      </c>
-      <c r="Z261" s="5">
-        <v>1200</v>
-      </c>
-      <c r="AA261" s="3">
-        <v>1200</v>
-      </c>
-      <c r="AB261" s="3">
-        <v>1100</v>
-      </c>
-      <c r="AC261" s="3">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="262" spans="1:29" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="262" spans="1:29" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>28</v>
       </c>
@@ -25745,7 +25748,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="263" spans="1:29" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:29" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>28</v>
       </c>
@@ -25835,7 +25838,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="264" spans="1:29" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:29" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>28</v>
       </c>
@@ -25925,7 +25928,7 @@
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="265" spans="1:29" s="27" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:29" s="27" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>28</v>
       </c>
@@ -26029,7 +26032,7 @@
         <v>3.0008124999999994</v>
       </c>
     </row>
-    <row r="266" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
         <v>28</v>
       </c>
@@ -26133,7 +26136,7 @@
         <v>3.0008124999999994</v>
       </c>
     </row>
-    <row r="267" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>28</v>
       </c>
@@ -26198,7 +26201,7 @@
       <c r="AB267" s="3"/>
       <c r="AC267" s="3"/>
     </row>
-    <row r="268" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>28</v>
       </c>
@@ -26263,7 +26266,7 @@
       <c r="AB268" s="3"/>
       <c r="AC268" s="3"/>
     </row>
-    <row r="269" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>28</v>
       </c>
@@ -26352,7 +26355,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="270" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>28</v>
       </c>
@@ -26441,7 +26444,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="271" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>28</v>
       </c>
@@ -26530,7 +26533,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="272" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
         <v>28</v>
       </c>
@@ -26619,7 +26622,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="273" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>28</v>
       </c>
@@ -26708,7 +26711,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="274" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
         <v>28</v>
       </c>
@@ -26797,7 +26800,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="275" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>28</v>
       </c>
@@ -26886,7 +26889,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="276" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
         <v>28</v>
       </c>
@@ -26981,7 +26984,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="277" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>28</v>
       </c>
@@ -27076,7 +27079,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="278" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
         <v>28</v>
       </c>
@@ -27171,7 +27174,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="279" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>28</v>
       </c>
@@ -27266,7 +27269,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="280" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
         <v>28</v>
       </c>
@@ -27361,7 +27364,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="281" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>28</v>
       </c>
@@ -27456,7 +27459,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="282" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
         <v>28</v>
       </c>
@@ -27551,7 +27554,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="283" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
         <v>28</v>
       </c>
@@ -27640,7 +27643,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="284" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
         <v>28</v>
       </c>
@@ -27705,7 +27708,7 @@
       <c r="AB284" s="5"/>
       <c r="AC284" s="5"/>
     </row>
-    <row r="285" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
         <v>28</v>
       </c>
@@ -27800,7 +27803,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="286" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
         <v>28</v>
       </c>
@@ -27889,7 +27892,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="287" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
         <v>28</v>
       </c>
@@ -27978,7 +27981,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="288" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
         <v>28</v>
       </c>
@@ -28067,7 +28070,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="289" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
         <v>28</v>
       </c>
@@ -28156,7 +28159,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="290" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
         <v>28</v>
       </c>
@@ -28245,7 +28248,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="291" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
         <v>28</v>
       </c>
@@ -28334,7 +28337,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="292" spans="1:29" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
         <v>28</v>
       </c>
@@ -28423,7 +28426,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="293" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
         <v>28</v>
       </c>
@@ -28488,7 +28491,7 @@
       <c r="AB293" s="3"/>
       <c r="AC293" s="3"/>
     </row>
-    <row r="294" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
         <v>28</v>
       </c>
@@ -28553,7 +28556,7 @@
       <c r="AB294" s="5"/>
       <c r="AC294" s="5"/>
     </row>
-    <row r="295" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
         <v>28</v>
       </c>
@@ -28618,7 +28621,7 @@
       <c r="AB295" s="3"/>
       <c r="AC295" s="3"/>
     </row>
-    <row r="296" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
         <v>28</v>
       </c>
@@ -28723,8 +28726,12 @@
   <autoFilter ref="A2:AC296">
     <filterColumn colId="4">
       <filters>
-        <filter val="fuel cell ancillary BoP mass per power"/>
-        <filter val="fuel cell essential BoP mass per power"/>
+        <filter val="battery cell energy density, LFP"/>
+        <filter val="battery cell energy density, LTO"/>
+        <filter val="battery cell energy density, NCA"/>
+        <filter val="battery cell energy density, NMC-111"/>
+        <filter val="battery cell power density"/>
+        <filter val="fuel cell power area density"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Set up Github Actions
</commit_message>
<xml_diff>
--- a/dev/Input data_truck.xlsx
+++ b/dev/Input data_truck.xlsx
@@ -1303,13 +1303,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AD296"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="11" ySplit="2" topLeftCell="L154" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J207" sqref="J207"/>
+      <selection pane="bottomRight" activeCell="R293" sqref="R293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1477,7 +1478,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1582,7 +1583,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1792,7 +1793,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1897,7 +1898,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -2099,7 +2100,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -2200,7 +2201,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -2265,7 +2266,7 @@
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -2338,7 +2339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -2548,7 +2549,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
@@ -2653,7 +2654,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="14.65" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -2758,7 +2759,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="14.65" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -2859,7 +2860,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -2960,7 +2961,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
@@ -3150,7 +3151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>943.11249999999995</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
@@ -3354,7 +3355,7 @@
         <v>1886.2249999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -3456,7 +3457,7 @@
         <v>3600.9749999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -3558,7 +3559,7 @@
         <v>3772.45</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -3660,7 +3661,7 @@
         <v>4115.3999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
@@ -3762,7 +3763,7 @@
         <v>4115.3999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -3864,7 +3865,7 @@
         <v>5658.6750000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>57</v>
       </c>
@@ -3965,7 +3966,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>57</v>
       </c>
@@ -4066,7 +4067,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
@@ -4167,7 +4168,7 @@
         <v>2.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>57</v>
       </c>
@@ -4268,7 +4269,7 @@
         <v>6.1199999999999991E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>57</v>
       </c>
@@ -4370,7 +4371,7 @@
       </c>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>57</v>
       </c>
@@ -4472,7 +4473,7 @@
       </c>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
@@ -4574,7 +4575,7 @@
       </c>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>57</v>
       </c>
@@ -4656,7 +4657,7 @@
       </c>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -4738,7 +4739,7 @@
       </c>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
@@ -4820,7 +4821,7 @@
       </c>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
@@ -4902,7 +4903,7 @@
       </c>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -4984,7 +4985,7 @@
       </c>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>57</v>
       </c>
@@ -5066,7 +5067,7 @@
       </c>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
@@ -5148,7 +5149,7 @@
       </c>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -5256,7 +5257,7 @@
       </c>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
@@ -5364,7 +5365,7 @@
       </c>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -5472,7 +5473,7 @@
       </c>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -5580,7 +5581,7 @@
       </c>
       <c r="AD44" s="1"/>
     </row>
-    <row r="45" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>57</v>
       </c>
@@ -5688,7 +5689,7 @@
       </c>
       <c r="AD45" s="1"/>
     </row>
-    <row r="46" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
@@ -5796,7 +5797,7 @@
       </c>
       <c r="AD46" s="1"/>
     </row>
-    <row r="47" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>57</v>
       </c>
@@ -5904,7 +5905,7 @@
       </c>
       <c r="AD47" s="1"/>
     </row>
-    <row r="48" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
@@ -6012,7 +6013,7 @@
       </c>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
@@ -6120,7 +6121,7 @@
       </c>
       <c r="AD49" s="1"/>
     </row>
-    <row r="50" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -6228,7 +6229,7 @@
       </c>
       <c r="AD50" s="1"/>
     </row>
-    <row r="51" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -6336,7 +6337,7 @@
       </c>
       <c r="AD51" s="1"/>
     </row>
-    <row r="52" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
@@ -6444,7 +6445,7 @@
       </c>
       <c r="AD52" s="1"/>
     </row>
-    <row r="53" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>57</v>
       </c>
@@ -6552,7 +6553,7 @@
       </c>
       <c r="AD53" s="1"/>
     </row>
-    <row r="54" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -6660,7 +6661,7 @@
       </c>
       <c r="AD54" s="1"/>
     </row>
-    <row r="55" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>57</v>
       </c>
@@ -6750,7 +6751,7 @@
       </c>
       <c r="AD55" s="1"/>
     </row>
-    <row r="56" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -6840,7 +6841,7 @@
       </c>
       <c r="AD56" s="1"/>
     </row>
-    <row r="57" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>57</v>
       </c>
@@ -6930,7 +6931,7 @@
       </c>
       <c r="AD57" s="1"/>
     </row>
-    <row r="58" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -7020,7 +7021,7 @@
       </c>
       <c r="AD58" s="1"/>
     </row>
-    <row r="59" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -7110,7 +7111,7 @@
       </c>
       <c r="AD59" s="1"/>
     </row>
-    <row r="60" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -7200,7 +7201,7 @@
       </c>
       <c r="AD60" s="1"/>
     </row>
-    <row r="61" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
@@ -7290,7 +7291,7 @@
       </c>
       <c r="AD61" s="1"/>
     </row>
-    <row r="62" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>57</v>
       </c>
@@ -7372,7 +7373,7 @@
       </c>
       <c r="AD62" s="1"/>
     </row>
-    <row r="63" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>57</v>
       </c>
@@ -7462,7 +7463,7 @@
       </c>
       <c r="AD63" s="1"/>
     </row>
-    <row r="64" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>57</v>
       </c>
@@ -7552,7 +7553,7 @@
       </c>
       <c r="AD64" s="1"/>
     </row>
-    <row r="65" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>57</v>
       </c>
@@ -7642,7 +7643,7 @@
       </c>
       <c r="AD65" s="1"/>
     </row>
-    <row r="66" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>57</v>
       </c>
@@ -7732,7 +7733,7 @@
       </c>
       <c r="AD66" s="1"/>
     </row>
-    <row r="67" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>57</v>
       </c>
@@ -7822,7 +7823,7 @@
       </c>
       <c r="AD67" s="1"/>
     </row>
-    <row r="68" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>57</v>
       </c>
@@ -7912,7 +7913,7 @@
       </c>
       <c r="AD68" s="1"/>
     </row>
-    <row r="69" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>57</v>
       </c>
@@ -8002,7 +8003,7 @@
       </c>
       <c r="AD69" s="1"/>
     </row>
-    <row r="70" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>57</v>
       </c>
@@ -8084,7 +8085,7 @@
       </c>
       <c r="AD70" s="1"/>
     </row>
-    <row r="71" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>57</v>
       </c>
@@ -8166,7 +8167,7 @@
       </c>
       <c r="AD71" s="1"/>
     </row>
-    <row r="72" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>57</v>
       </c>
@@ -8254,7 +8255,7 @@
       </c>
       <c r="AD72" s="1"/>
     </row>
-    <row r="73" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>57</v>
       </c>
@@ -8336,7 +8337,7 @@
       </c>
       <c r="AD73" s="1"/>
     </row>
-    <row r="74" spans="1:30" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
@@ -8444,7 +8445,7 @@
       </c>
       <c r="AD74" s="1"/>
     </row>
-    <row r="75" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
@@ -8526,7 +8527,7 @@
       </c>
       <c r="AD75" s="1"/>
     </row>
-    <row r="76" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>57</v>
       </c>
@@ -8608,7 +8609,7 @@
       </c>
       <c r="AD76" s="1"/>
     </row>
-    <row r="77" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>57</v>
       </c>
@@ -8690,7 +8691,7 @@
       </c>
       <c r="AD77" s="1"/>
     </row>
-    <row r="78" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>57</v>
       </c>
@@ -8772,7 +8773,7 @@
       </c>
       <c r="AD78" s="1"/>
     </row>
-    <row r="79" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>57</v>
       </c>
@@ -8854,7 +8855,7 @@
       </c>
       <c r="AD79" s="1"/>
     </row>
-    <row r="80" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>57</v>
       </c>
@@ -8936,7 +8937,7 @@
       </c>
       <c r="AD80" s="1"/>
     </row>
-    <row r="81" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>57</v>
       </c>
@@ -9018,7 +9019,7 @@
       </c>
       <c r="AD81" s="1"/>
     </row>
-    <row r="82" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>57</v>
       </c>
@@ -9076,7 +9077,7 @@
       </c>
       <c r="AD82" s="1"/>
     </row>
-    <row r="83" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>57</v>
       </c>
@@ -9158,7 +9159,7 @@
       </c>
       <c r="AD83" s="1"/>
     </row>
-    <row r="84" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>57</v>
       </c>
@@ -9240,7 +9241,7 @@
       </c>
       <c r="AD84" s="1"/>
     </row>
-    <row r="85" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>57</v>
       </c>
@@ -9322,7 +9323,7 @@
       </c>
       <c r="AD85" s="1"/>
     </row>
-    <row r="86" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>57</v>
       </c>
@@ -9404,7 +9405,7 @@
       </c>
       <c r="AD86" s="1"/>
     </row>
-    <row r="87" spans="1:30" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>57</v>
       </c>
@@ -9494,7 +9495,7 @@
       </c>
       <c r="AD87" s="1"/>
     </row>
-    <row r="88" spans="1:30" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>57</v>
       </c>
@@ -9584,7 +9585,7 @@
       </c>
       <c r="AD88" s="1"/>
     </row>
-    <row r="89" spans="1:30" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>57</v>
       </c>
@@ -9674,7 +9675,7 @@
       </c>
       <c r="AD89" s="1"/>
     </row>
-    <row r="90" spans="1:30" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>57</v>
       </c>
@@ -9764,7 +9765,7 @@
       </c>
       <c r="AD90" s="1"/>
     </row>
-    <row r="91" spans="1:30" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>57</v>
       </c>
@@ -9854,7 +9855,7 @@
       </c>
       <c r="AD91" s="1"/>
     </row>
-    <row r="92" spans="1:30" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:30" s="24" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>57</v>
       </c>
@@ -9944,7 +9945,7 @@
       </c>
       <c r="AD92" s="1"/>
     </row>
-    <row r="93" spans="1:30" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:30" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>57</v>
       </c>
@@ -10026,7 +10027,7 @@
       </c>
       <c r="AD93" s="1"/>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>57</v>
       </c>
@@ -10113,7 +10114,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>35</v>
       </c>
@@ -10214,7 +10215,7 @@
         <v>180000</v>
       </c>
     </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>35</v>
       </c>
@@ -10315,7 +10316,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>35</v>
       </c>
@@ -10416,7 +10417,7 @@
         <v>1050000</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>35</v>
       </c>
@@ -10517,7 +10518,7 @@
         <v>875000</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>35</v>
       </c>
@@ -10618,7 +10619,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>35</v>
       </c>
@@ -10719,7 +10720,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>35</v>
       </c>
@@ -10820,7 +10821,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>35</v>
       </c>
@@ -10921,7 +10922,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>35</v>
       </c>
@@ -11022,7 +11023,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>35</v>
       </c>
@@ -11123,7 +11124,7 @@
         <v>52500</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>35</v>
       </c>
@@ -11224,7 +11225,7 @@
         <v>43750</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>35</v>
       </c>
@@ -11325,7 +11326,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>35</v>
       </c>
@@ -11426,7 +11427,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>35</v>
       </c>
@@ -11527,7 +11528,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>37</v>
       </c>
@@ -11614,7 +11615,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>37</v>
       </c>
@@ -11705,7 +11706,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>37</v>
       </c>
@@ -11790,7 +11791,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>37</v>
       </c>
@@ -11875,7 +11876,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>30</v>
       </c>
@@ -11936,7 +11937,7 @@
       <c r="AB113" s="5"/>
       <c r="AC113" s="5"/>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>30</v>
       </c>
@@ -11997,7 +11998,7 @@
       <c r="AB114" s="5"/>
       <c r="AC114" s="5"/>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>30</v>
       </c>
@@ -12058,7 +12059,7 @@
       <c r="AB115" s="5"/>
       <c r="AC115" s="5"/>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>30</v>
       </c>
@@ -12147,7 +12148,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>30</v>
       </c>
@@ -12232,7 +12233,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="118" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>30</v>
       </c>
@@ -12321,7 +12322,7 @@
         <v>27500</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>30</v>
       </c>
@@ -12406,7 +12407,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>30</v>
       </c>
@@ -12495,7 +12496,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>30</v>
       </c>
@@ -12584,7 +12585,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>30</v>
       </c>
@@ -12683,7 +12684,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>30</v>
       </c>
@@ -12782,7 +12783,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>30</v>
       </c>
@@ -12884,7 +12885,7 @@
         <v>11646.250000000004</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>30</v>
       </c>
@@ -12986,7 +12987,7 @@
         <v>11646.250000000004</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>30</v>
       </c>
@@ -13075,7 +13076,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>30</v>
       </c>
@@ -13170,7 +13171,7 @@
         <v>0.94760000000000011</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>30</v>
       </c>
@@ -13265,7 +13266,7 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>30</v>
       </c>
@@ -13354,7 +13355,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>30</v>
       </c>
@@ -13443,7 +13444,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>30</v>
       </c>
@@ -13532,7 +13533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>30</v>
       </c>
@@ -13621,7 +13622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>30</v>
       </c>
@@ -13716,7 +13717,7 @@
         <v>3.4499999999999997</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>30</v>
       </c>
@@ -13805,7 +13806,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>30</v>
       </c>
@@ -13894,7 +13895,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>30</v>
       </c>
@@ -13983,7 +13984,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>30</v>
       </c>
@@ -14070,7 +14071,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>30</v>
       </c>
@@ -14157,7 +14158,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>30</v>
       </c>
@@ -14256,7 +14257,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>30</v>
       </c>
@@ -14355,7 +14356,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="23" t="s">
         <v>27</v>
       </c>
@@ -14417,7 +14418,7 @@
       <c r="AB141" s="19"/>
       <c r="AC141" s="19"/>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="23" t="s">
         <v>27</v>
       </c>
@@ -14479,7 +14480,7 @@
       <c r="AB142" s="19"/>
       <c r="AC142" s="19"/>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="23" t="s">
         <v>27</v>
       </c>
@@ -14541,7 +14542,7 @@
       <c r="AB143" s="19"/>
       <c r="AC143" s="19"/>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23" t="s">
         <v>27</v>
       </c>
@@ -14603,7 +14604,7 @@
       <c r="AB144" s="19"/>
       <c r="AC144" s="19"/>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="23" t="s">
         <v>27</v>
       </c>
@@ -14665,7 +14666,7 @@
       <c r="AB145" s="19"/>
       <c r="AC145" s="19"/>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="23" t="s">
         <v>27</v>
       </c>
@@ -14727,7 +14728,7 @@
       <c r="AB146" s="19"/>
       <c r="AC146" s="19"/>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="23" t="s">
         <v>27</v>
       </c>
@@ -14789,7 +14790,7 @@
       <c r="AB147" s="19"/>
       <c r="AC147" s="19"/>
     </row>
-    <row r="148" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="23" t="s">
         <v>27</v>
       </c>
@@ -14890,7 +14891,7 @@
         <v>242.5</v>
       </c>
     </row>
-    <row r="149" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="23" t="s">
         <v>27</v>
       </c>
@@ -14991,7 +14992,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="23" t="s">
         <v>27</v>
       </c>
@@ -15092,7 +15093,7 @@
         <v>1247.5</v>
       </c>
     </row>
-    <row r="151" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="23" t="s">
         <v>27</v>
       </c>
@@ -15194,7 +15195,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="152" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="23" t="s">
         <v>27</v>
       </c>
@@ -15295,7 +15296,7 @@
         <v>1422.5</v>
       </c>
     </row>
-    <row r="153" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="23" t="s">
         <v>27</v>
       </c>
@@ -15396,7 +15397,7 @@
         <v>1777.5</v>
       </c>
     </row>
-    <row r="154" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="23" t="s">
         <v>27</v>
       </c>
@@ -15497,7 +15498,7 @@
         <v>2666.25</v>
       </c>
     </row>
-    <row r="155" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="23" t="s">
         <v>27</v>
       </c>
@@ -15598,7 +15599,7 @@
         <v>387.5</v>
       </c>
     </row>
-    <row r="156" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="23" t="s">
         <v>27</v>
       </c>
@@ -15699,7 +15700,7 @@
         <v>831.25</v>
       </c>
     </row>
-    <row r="157" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="23" t="s">
         <v>27</v>
       </c>
@@ -15800,7 +15801,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="158" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="23" t="s">
         <v>27</v>
       </c>
@@ -15902,7 +15903,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="159" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="23" t="s">
         <v>27</v>
       </c>
@@ -16003,7 +16004,7 @@
         <v>2656.25</v>
       </c>
     </row>
-    <row r="160" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="23" t="s">
         <v>27</v>
       </c>
@@ -16104,7 +16105,7 @@
         <v>3320</v>
       </c>
     </row>
-    <row r="161" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="23" t="s">
         <v>27</v>
       </c>
@@ -16205,7 +16206,7 @@
         <v>4980</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="23" t="s">
         <v>27</v>
       </c>
@@ -16292,7 +16293,7 @@
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="23" t="s">
         <v>27</v>
       </c>
@@ -16381,7 +16382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="23" t="s">
         <v>27</v>
       </c>
@@ -16470,7 +16471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="23" t="s">
         <v>27</v>
       </c>
@@ -16559,7 +16560,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="23" t="s">
         <v>27</v>
       </c>
@@ -16648,7 +16649,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="23" t="s">
         <v>27</v>
       </c>
@@ -16737,7 +16738,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="23" t="s">
         <v>27</v>
       </c>
@@ -16826,7 +16827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="23" t="s">
         <v>27</v>
       </c>
@@ -16915,7 +16916,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="23" t="s">
         <v>27</v>
       </c>
@@ -17022,7 +17023,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="23" t="s">
         <v>27</v>
       </c>
@@ -17129,7 +17130,7 @@
         <v>34.4</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="23" t="s">
         <v>27</v>
       </c>
@@ -17230,7 +17231,7 @@
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="23" t="s">
         <v>27</v>
       </c>
@@ -17331,7 +17332,7 @@
         <v>31.200000000000003</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="23" t="s">
         <v>27</v>
       </c>
@@ -17432,7 +17433,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="23" t="s">
         <v>27</v>
       </c>
@@ -17533,7 +17534,7 @@
         <v>26.400000000000002</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="23" t="s">
         <v>27</v>
       </c>
@@ -17634,7 +17635,7 @@
         <v>19.200000000000003</v>
       </c>
     </row>
-    <row r="177" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="23" t="s">
         <v>27</v>
       </c>
@@ -17735,7 +17736,7 @@
         <v>148.75</v>
       </c>
     </row>
-    <row r="178" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="23" t="s">
         <v>27</v>
       </c>
@@ -17836,7 +17837,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="179" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="23" t="s">
         <v>27</v>
       </c>
@@ -17937,7 +17938,7 @@
         <v>767.5</v>
       </c>
     </row>
-    <row r="180" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="23" t="s">
         <v>27</v>
       </c>
@@ -18039,7 +18040,7 @@
         <v>3125</v>
       </c>
     </row>
-    <row r="181" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="23" t="s">
         <v>27</v>
       </c>
@@ -18140,7 +18141,7 @@
         <v>1058.75</v>
       </c>
     </row>
-    <row r="182" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="23" t="s">
         <v>27</v>
       </c>
@@ -18241,7 +18242,7 @@
         <v>1323.75</v>
       </c>
     </row>
-    <row r="183" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="23" t="s">
         <v>27</v>
       </c>
@@ -18342,7 +18343,7 @@
         <v>5062.5</v>
       </c>
     </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="23" t="s">
         <v>27</v>
       </c>
@@ -18431,7 +18432,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="23" t="s">
         <v>27</v>
       </c>
@@ -18520,7 +18521,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="23" t="s">
         <v>27</v>
       </c>
@@ -18609,7 +18610,7 @@
         <v>10900</v>
       </c>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="23" t="s">
         <v>27</v>
       </c>
@@ -18698,7 +18699,7 @@
         <v>16400</v>
       </c>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="23" t="s">
         <v>27</v>
       </c>
@@ -18787,7 +18788,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="23" t="s">
         <v>27</v>
       </c>
@@ -18876,7 +18877,7 @@
         <v>28100</v>
       </c>
     </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="23" t="s">
         <v>27</v>
       </c>
@@ -18965,7 +18966,7 @@
         <v>39000</v>
       </c>
     </row>
-    <row r="191" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="23" t="s">
         <v>27</v>
       </c>
@@ -19062,7 +19063,7 @@
         <v>0.35000000000000003</v>
       </c>
     </row>
-    <row r="192" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="23" t="s">
         <v>27</v>
       </c>
@@ -19159,7 +19160,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="193" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>27</v>
       </c>
@@ -19220,7 +19221,7 @@
       <c r="AB193" s="4"/>
       <c r="AC193" s="4"/>
     </row>
-    <row r="194" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>27</v>
       </c>
@@ -19281,7 +19282,7 @@
       <c r="AB194" s="4"/>
       <c r="AC194" s="4"/>
     </row>
-    <row r="195" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>27</v>
       </c>
@@ -19342,7 +19343,7 @@
       <c r="AB195" s="4"/>
       <c r="AC195" s="4"/>
     </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>27</v>
       </c>
@@ -19403,7 +19404,7 @@
       <c r="AB196" s="4"/>
       <c r="AC196" s="4"/>
     </row>
-    <row r="197" spans="1:29" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:29" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>27</v>
       </c>
@@ -19464,7 +19465,7 @@
       <c r="AB197" s="4"/>
       <c r="AC197" s="4"/>
     </row>
-    <row r="198" spans="1:29" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:29" ht="29.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>27</v>
       </c>
@@ -19525,7 +19526,7 @@
       <c r="AB198" s="4"/>
       <c r="AC198" s="4"/>
     </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>27</v>
       </c>
@@ -19586,7 +19587,7 @@
       <c r="AB199" s="4"/>
       <c r="AC199" s="4"/>
     </row>
-    <row r="200" spans="1:29" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:29" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="23" t="s">
         <v>27</v>
       </c>
@@ -19692,7 +19693,7 @@
         <v>878.75</v>
       </c>
     </row>
-    <row r="201" spans="1:29" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:29" ht="26.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="23" t="s">
         <v>27</v>
       </c>
@@ -19798,7 +19799,7 @@
         <v>1882.5</v>
       </c>
     </row>
-    <row r="202" spans="1:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:29" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="23" t="s">
         <v>27</v>
       </c>
@@ -19905,7 +19906,7 @@
         <v>4518.75</v>
       </c>
     </row>
-    <row r="203" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="23" t="s">
         <v>27</v>
       </c>
@@ -20008,7 +20009,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="204" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="23" t="s">
         <v>27</v>
       </c>
@@ -20115,7 +20116,7 @@
         <v>5538.75</v>
       </c>
     </row>
-    <row r="205" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="23" t="s">
         <v>27</v>
       </c>
@@ -20222,7 +20223,7 @@
         <v>6923.75</v>
       </c>
     </row>
-    <row r="206" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="23" t="s">
         <v>27</v>
       </c>
@@ -20329,7 +20330,7 @@
         <v>10386.25</v>
       </c>
     </row>
-    <row r="207" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="23" t="s">
         <v>27</v>
       </c>
@@ -20427,7 +20428,7 @@
         <v>3.8581874999999992</v>
       </c>
     </row>
-    <row r="208" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="23" t="s">
         <v>27</v>
       </c>
@@ -20525,7 +20526,7 @@
         <v>5.4871999999999996</v>
       </c>
     </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="23" t="s">
         <v>27</v>
       </c>
@@ -20623,7 +20624,7 @@
         <v>6.6875249999999982</v>
       </c>
     </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="23" t="s">
         <v>27</v>
       </c>
@@ -20721,7 +20722,7 @@
         <v>6.6875249999999982</v>
       </c>
     </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="23" t="s">
         <v>27</v>
       </c>
@@ -20810,7 +20811,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="23" t="s">
         <v>27</v>
       </c>
@@ -20908,7 +20909,7 @@
         <v>7.2019499999999992</v>
       </c>
     </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="23" t="s">
         <v>27</v>
       </c>
@@ -21006,7 +21007,7 @@
         <v>7.2019499999999992</v>
       </c>
     </row>
-    <row r="214" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="23" t="s">
         <v>27</v>
       </c>
@@ -21107,7 +21108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="215" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="23" t="s">
         <v>27</v>
       </c>
@@ -21208,7 +21209,7 @@
         <v>117.5</v>
       </c>
     </row>
-    <row r="216" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="23" t="s">
         <v>27</v>
       </c>
@@ -21309,7 +21310,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="217" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="23" t="s">
         <v>27</v>
       </c>
@@ -21411,7 +21412,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="218" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:29" ht="15.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="23" t="s">
         <v>27</v>
       </c>
@@ -21512,7 +21513,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="219" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="23" t="s">
         <v>27</v>
       </c>
@@ -21613,7 +21614,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="220" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="23" t="s">
         <v>27</v>
       </c>
@@ -21714,7 +21715,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="221" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="23" t="s">
         <v>27</v>
       </c>
@@ -21815,7 +21816,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="222" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="23" t="s">
         <v>27</v>
       </c>
@@ -21916,7 +21917,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="223" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="23" t="s">
         <v>27</v>
       </c>
@@ -22017,7 +22018,7 @@
         <v>156.25</v>
       </c>
     </row>
-    <row r="224" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="23" t="s">
         <v>27</v>
       </c>
@@ -22119,7 +22120,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="225" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="23" t="s">
         <v>27</v>
       </c>
@@ -22220,7 +22221,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="226" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="23" t="s">
         <v>27</v>
       </c>
@@ -22321,7 +22322,7 @@
         <v>331.25</v>
       </c>
     </row>
-    <row r="227" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="23" t="s">
         <v>27</v>
       </c>
@@ -22422,7 +22423,7 @@
         <v>497.5</v>
       </c>
     </row>
-    <row r="228" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="23" t="s">
         <v>27</v>
       </c>
@@ -22523,7 +22524,7 @@
         <v>0.37400000000000005</v>
       </c>
     </row>
-    <row r="229" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="23" t="s">
         <v>27</v>
       </c>
@@ -22624,7 +22625,7 @@
         <v>0.22000000000000003</v>
       </c>
     </row>
-    <row r="230" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>27</v>
       </c>
@@ -22725,7 +22726,7 @@
         <v>0.35200000000000004</v>
       </c>
     </row>
-    <row r="231" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>27</v>
       </c>
@@ -22826,7 +22827,7 @@
         <v>0.50600000000000012</v>
       </c>
     </row>
-    <row r="232" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>27</v>
       </c>
@@ -22927,7 +22928,7 @@
         <v>0.49500000000000005</v>
       </c>
     </row>
-    <row r="233" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>27</v>
       </c>
@@ -23028,7 +23029,7 @@
         <v>0.38500000000000001</v>
       </c>
     </row>
-    <row r="234" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>27</v>
       </c>
@@ -23129,7 +23130,7 @@
         <v>0.38500000000000001</v>
       </c>
     </row>
-    <row r="235" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="23" t="s">
         <v>27</v>
       </c>
@@ -23230,7 +23231,7 @@
         <v>218.75</v>
       </c>
     </row>
-    <row r="236" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="23" t="s">
         <v>27</v>
       </c>
@@ -23331,7 +23332,7 @@
         <v>468.75</v>
       </c>
     </row>
-    <row r="237" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="23" t="s">
         <v>27</v>
       </c>
@@ -23432,7 +23433,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="238" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="23" t="s">
         <v>27</v>
       </c>
@@ -23534,7 +23535,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="239" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="23" t="s">
         <v>27</v>
       </c>
@@ -23635,7 +23636,7 @@
         <v>1152.5</v>
       </c>
     </row>
-    <row r="240" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="23" t="s">
         <v>27</v>
       </c>
@@ -23736,7 +23737,7 @@
         <v>1441.25</v>
       </c>
     </row>
-    <row r="241" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="23" t="s">
         <v>27</v>
       </c>
@@ -23837,7 +23838,7 @@
         <v>2162.5</v>
       </c>
     </row>
-    <row r="242" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="23" t="s">
         <v>27</v>
       </c>
@@ -23938,7 +23939,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="243" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="23" t="s">
         <v>27</v>
       </c>
@@ -24039,7 +24040,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="244" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="23" t="s">
         <v>27</v>
       </c>
@@ -24140,7 +24141,7 @@
         <v>156.25</v>
       </c>
     </row>
-    <row r="245" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="23" t="s">
         <v>27</v>
       </c>
@@ -24242,7 +24243,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="246" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="23" t="s">
         <v>27</v>
       </c>
@@ -24343,7 +24344,7 @@
         <v>783.75</v>
       </c>
     </row>
-    <row r="247" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="23" t="s">
         <v>27</v>
       </c>
@@ -24444,7 +24445,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="248" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="23" t="s">
         <v>27</v>
       </c>
@@ -24545,7 +24546,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="249" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="23" t="s">
         <v>27</v>
       </c>
@@ -24608,7 +24609,7 @@
       <c r="AB249" s="5"/>
       <c r="AC249" s="5"/>
     </row>
-    <row r="250" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="23" t="s">
         <v>27</v>
       </c>
@@ -24695,7 +24696,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="251" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="23" t="s">
         <v>27</v>
       </c>
@@ -24782,7 +24783,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="252" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
         <v>28</v>
       </c>
@@ -24883,7 +24884,7 @@
         <v>25.960000000000004</v>
       </c>
     </row>
-    <row r="253" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
         <v>28</v>
       </c>
@@ -24984,7 +24985,7 @@
         <v>15.400000000000002</v>
       </c>
     </row>
-    <row r="254" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>28</v>
       </c>
@@ -25081,7 +25082,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="255" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>28</v>
       </c>
@@ -25176,7 +25177,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="256" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>28</v>
       </c>
@@ -25269,7 +25270,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="257" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>28</v>
       </c>
@@ -25366,7 +25367,7 @@
         <v>5.5000000000000007E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
         <v>28</v>
       </c>
@@ -25469,7 +25470,7 @@
         <v>5.5000000000000007E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:29" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>28</v>
       </c>
@@ -25558,7 +25559,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="260" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:29" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
         <v>28</v>
       </c>
@@ -25665,7 +25666,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="261" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:29" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>28</v>
       </c>
@@ -25754,7 +25755,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="262" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:29" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>28</v>
       </c>
@@ -25835,7 +25836,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="263" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:29" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>28</v>
       </c>
@@ -25925,7 +25926,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="264" spans="1:29" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:29" s="26" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>28</v>
       </c>
@@ -26015,7 +26016,7 @@
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="265" spans="1:29" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:29" s="26" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>28</v>
       </c>
@@ -26119,7 +26120,7 @@
         <v>3.0008124999999994</v>
       </c>
     </row>
-    <row r="266" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
         <v>28</v>
       </c>
@@ -26223,7 +26224,7 @@
         <v>3.0008124999999994</v>
       </c>
     </row>
-    <row r="267" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>28</v>
       </c>
@@ -26288,7 +26289,7 @@
       <c r="AB267" s="3"/>
       <c r="AC267" s="3"/>
     </row>
-    <row r="268" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>28</v>
       </c>
@@ -26353,7 +26354,7 @@
       <c r="AB268" s="3"/>
       <c r="AC268" s="3"/>
     </row>
-    <row r="269" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>28</v>
       </c>
@@ -26442,7 +26443,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="270" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>28</v>
       </c>
@@ -26531,7 +26532,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="271" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>28</v>
       </c>
@@ -26620,7 +26621,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="272" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
         <v>28</v>
       </c>
@@ -26709,7 +26710,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="273" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>28</v>
       </c>
@@ -26798,7 +26799,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="274" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
         <v>28</v>
       </c>
@@ -26887,7 +26888,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="275" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>28</v>
       </c>
@@ -26976,7 +26977,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="276" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
         <v>28</v>
       </c>
@@ -27071,7 +27072,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="277" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>28</v>
       </c>
@@ -27166,7 +27167,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="278" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
         <v>28</v>
       </c>
@@ -27261,7 +27262,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="279" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>28</v>
       </c>
@@ -27356,7 +27357,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="280" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
         <v>28</v>
       </c>
@@ -27451,7 +27452,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="281" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>28</v>
       </c>
@@ -27546,7 +27547,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="282" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
         <v>28</v>
       </c>
@@ -27641,7 +27642,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="283" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
         <v>28</v>
       </c>
@@ -27730,7 +27731,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="284" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
         <v>28</v>
       </c>
@@ -27795,7 +27796,7 @@
       <c r="AB284" s="5"/>
       <c r="AC284" s="5"/>
     </row>
-    <row r="285" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
         <v>28</v>
       </c>
@@ -28708,7 +28709,7 @@
       <c r="AB295" s="3"/>
       <c r="AC295" s="3"/>
     </row>
-    <row r="296" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
         <v>28</v>
       </c>
@@ -28810,7 +28811,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AC296"/>
+  <autoFilter ref="A2:AC296">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="combustion power share"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I251" r:id="rId1"/>

</xml_diff>